<commit_message>
Did improvements with Find Linked Objects actions
</commit_message>
<xml_diff>
--- a/misc/xlsx_template.xlsx
+++ b/misc/xlsx_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="16155" windowHeight="6660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="18075" windowHeight="8700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,7 +31,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,11 +65,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>

</xml_diff>